<commit_message>
Author             : Prateek Kapoor File Modified      : WRS - BSC (SCGJ Work).xlsx Description        : updated with new suggestions from SCGJ
</commit_message>
<xml_diff>
--- a/Billing/Work Record Sheet/September/WRS - BSC (SCGJ Work).xlsx
+++ b/Billing/Work Record Sheet/September/WRS - BSC (SCGJ Work).xlsx
@@ -5,10 +5,10 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Prateek Kapoor\Google Drive (internship.smaltandberyl@gmail.com)\SCGJ MSA Details\Excel Sheet\Work Record Sheet\September\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Prateek Kapoor\Desktop\NSKFDC-App.git\trunk\Billing\Work Record Sheet\September\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{55B9FA85-3749-4A89-9F4E-11CC1C5A4E1E}" xr6:coauthVersionLast="37" xr6:coauthVersionMax="37" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DB49B734-701E-4174-B255-3648B3237345}" xr6:coauthVersionLast="37" xr6:coauthVersionMax="37" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="8240" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="80" uniqueCount="49">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="87" uniqueCount="53">
   <si>
     <t>S.No</t>
   </si>
@@ -172,6 +172,18 @@
   </si>
   <si>
     <t>Template image of SCGJ logo should navigate to SCGJ's website</t>
+  </si>
+  <si>
+    <t>Candidate Id should also be generated by the system in the excel sheet for 50 candidates</t>
+  </si>
+  <si>
+    <t>NA-411</t>
+  </si>
+  <si>
+    <t>NA-432</t>
+  </si>
+  <si>
+    <t>Add columns to candidate excel sheet as per Krishna's mail</t>
   </si>
 </sst>
 </file>
@@ -339,18 +351,6 @@
   <cellXfs count="15">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -370,6 +370,18 @@
     <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="6" fillId="4" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
   </cellXfs>
@@ -684,11 +696,11 @@
   <sheetPr>
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
-  <dimension ref="A1:F23"/>
+  <dimension ref="A1:F25"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B1" zoomScale="40" zoomScaleNormal="40" workbookViewId="0">
+    <sheetView tabSelected="1" zoomScale="40" zoomScaleNormal="40" workbookViewId="0">
       <pane ySplit="4" topLeftCell="A5" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="C15" sqref="C15"/>
+      <selection pane="bottomLeft" activeCell="A20" sqref="A20:A24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="46" x14ac:dyDescent="1"/>
@@ -697,430 +709,468 @@
     <col min="2" max="2" width="23.26953125" style="1" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="255.6328125" style="1" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="51" style="1" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="39.1796875" style="6" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="39.1796875" style="2" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="29" style="1" customWidth="1"/>
     <col min="7" max="7" width="11" style="1" bestFit="1" customWidth="1"/>
     <col min="8" max="16384" width="8.7265625" style="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:6" x14ac:dyDescent="1">
-      <c r="A1" s="2" t="s">
+      <c r="A1" s="11" t="s">
         <v>10</v>
       </c>
-      <c r="B1" s="2"/>
-      <c r="C1" s="2"/>
-      <c r="D1" s="2"/>
-      <c r="E1" s="2"/>
-      <c r="F1" s="2"/>
+      <c r="B1" s="11"/>
+      <c r="C1" s="11"/>
+      <c r="D1" s="11"/>
+      <c r="E1" s="11"/>
+      <c r="F1" s="11"/>
     </row>
     <row r="2" spans="1:6" x14ac:dyDescent="1">
-      <c r="A2" s="2"/>
-      <c r="B2" s="2"/>
-      <c r="C2" s="2"/>
-      <c r="D2" s="2"/>
-      <c r="E2" s="2"/>
-      <c r="F2" s="2"/>
+      <c r="A2" s="11"/>
+      <c r="B2" s="11"/>
+      <c r="C2" s="11"/>
+      <c r="D2" s="11"/>
+      <c r="E2" s="11"/>
+      <c r="F2" s="11"/>
     </row>
     <row r="3" spans="1:6" x14ac:dyDescent="1">
-      <c r="A3" s="3"/>
-      <c r="B3" s="4"/>
-      <c r="C3" s="4"/>
-      <c r="D3" s="4"/>
-      <c r="E3" s="4"/>
-      <c r="F3" s="5"/>
+      <c r="A3" s="12"/>
+      <c r="B3" s="13"/>
+      <c r="C3" s="13"/>
+      <c r="D3" s="13"/>
+      <c r="E3" s="13"/>
+      <c r="F3" s="14"/>
     </row>
     <row r="4" spans="1:6" x14ac:dyDescent="1">
-      <c r="A4" s="7" t="s">
+      <c r="A4" s="3" t="s">
         <v>0</v>
       </c>
-      <c r="B4" s="7" t="s">
+      <c r="B4" s="3" t="s">
         <v>1</v>
       </c>
-      <c r="C4" s="7" t="s">
+      <c r="C4" s="3" t="s">
         <v>2</v>
       </c>
-      <c r="D4" s="7" t="s">
+      <c r="D4" s="3" t="s">
         <v>4</v>
       </c>
-      <c r="E4" s="7" t="s">
+      <c r="E4" s="3" t="s">
         <v>5</v>
       </c>
-      <c r="F4" s="7" t="s">
+      <c r="F4" s="3" t="s">
         <v>3</v>
       </c>
     </row>
     <row r="5" spans="1:6" x14ac:dyDescent="1">
-      <c r="A5" s="8">
+      <c r="A5" s="4">
         <v>1</v>
       </c>
-      <c r="B5" s="9" t="s">
+      <c r="B5" s="5" t="s">
         <v>23</v>
       </c>
-      <c r="C5" s="9" t="s">
+      <c r="C5" s="5" t="s">
         <v>11</v>
       </c>
-      <c r="D5" s="8" t="s">
+      <c r="D5" s="4" t="s">
         <v>6</v>
       </c>
-      <c r="E5" s="10">
-        <v>8</v>
-      </c>
-      <c r="F5" s="11" t="s">
+      <c r="E5" s="6">
+        <v>8</v>
+      </c>
+      <c r="F5" s="7" t="s">
         <v>7</v>
       </c>
     </row>
     <row r="6" spans="1:6" x14ac:dyDescent="1">
-      <c r="A6" s="8">
+      <c r="A6" s="4">
         <v>2</v>
       </c>
-      <c r="B6" s="9" t="s">
+      <c r="B6" s="5" t="s">
         <v>24</v>
       </c>
-      <c r="C6" s="9" t="s">
+      <c r="C6" s="5" t="s">
         <v>12</v>
       </c>
-      <c r="D6" s="8" t="s">
+      <c r="D6" s="4" t="s">
         <v>6</v>
       </c>
-      <c r="E6" s="10">
+      <c r="E6" s="6">
         <v>2</v>
       </c>
-      <c r="F6" s="11" t="s">
+      <c r="F6" s="7" t="s">
         <v>7</v>
       </c>
     </row>
     <row r="7" spans="1:6" x14ac:dyDescent="1">
-      <c r="A7" s="8">
+      <c r="A7" s="4">
         <v>3</v>
       </c>
-      <c r="B7" s="9" t="s">
+      <c r="B7" s="5" t="s">
         <v>25</v>
       </c>
-      <c r="C7" s="9" t="s">
+      <c r="C7" s="5" t="s">
         <v>13</v>
       </c>
-      <c r="D7" s="8" t="s">
-        <v>8</v>
-      </c>
-      <c r="E7" s="10">
+      <c r="D7" s="4" t="s">
+        <v>8</v>
+      </c>
+      <c r="E7" s="6">
         <v>1</v>
       </c>
-      <c r="F7" s="11" t="s">
+      <c r="F7" s="7" t="s">
         <v>7</v>
       </c>
     </row>
     <row r="8" spans="1:6" x14ac:dyDescent="1">
-      <c r="A8" s="8">
+      <c r="A8" s="4">
         <v>4</v>
       </c>
-      <c r="B8" s="9" t="s">
+      <c r="B8" s="5" t="s">
         <v>26</v>
       </c>
-      <c r="C8" s="9" t="s">
+      <c r="C8" s="5" t="s">
         <v>14</v>
       </c>
-      <c r="D8" s="8" t="s">
-        <v>8</v>
-      </c>
-      <c r="E8" s="10">
-        <v>8</v>
-      </c>
-      <c r="F8" s="11" t="s">
+      <c r="D8" s="4" t="s">
+        <v>8</v>
+      </c>
+      <c r="E8" s="6">
+        <v>8</v>
+      </c>
+      <c r="F8" s="7" t="s">
         <v>7</v>
       </c>
     </row>
     <row r="9" spans="1:6" x14ac:dyDescent="1">
-      <c r="A9" s="8">
+      <c r="A9" s="4">
         <v>5</v>
       </c>
-      <c r="B9" s="9" t="s">
+      <c r="B9" s="5" t="s">
         <v>27</v>
       </c>
-      <c r="C9" s="9" t="s">
+      <c r="C9" s="5" t="s">
         <v>15</v>
       </c>
-      <c r="D9" s="8" t="s">
-        <v>8</v>
-      </c>
-      <c r="E9" s="10">
-        <v>8</v>
-      </c>
-      <c r="F9" s="11" t="s">
+      <c r="D9" s="4" t="s">
+        <v>8</v>
+      </c>
+      <c r="E9" s="6">
+        <v>8</v>
+      </c>
+      <c r="F9" s="7" t="s">
         <v>7</v>
       </c>
     </row>
     <row r="10" spans="1:6" x14ac:dyDescent="1">
-      <c r="A10" s="8">
+      <c r="A10" s="4">
         <v>6</v>
       </c>
-      <c r="B10" s="9" t="s">
+      <c r="B10" s="5" t="s">
         <v>28</v>
       </c>
-      <c r="C10" s="9" t="s">
+      <c r="C10" s="5" t="s">
         <v>16</v>
       </c>
-      <c r="D10" s="8" t="s">
+      <c r="D10" s="4" t="s">
         <v>6</v>
       </c>
-      <c r="E10" s="10">
+      <c r="E10" s="6">
         <v>4</v>
       </c>
-      <c r="F10" s="11" t="s">
+      <c r="F10" s="7" t="s">
         <v>7</v>
       </c>
     </row>
     <row r="11" spans="1:6" x14ac:dyDescent="1">
-      <c r="A11" s="8">
-        <v>7</v>
-      </c>
-      <c r="B11" s="9" t="s">
+      <c r="A11" s="4">
+        <v>7</v>
+      </c>
+      <c r="B11" s="5" t="s">
         <v>29</v>
       </c>
-      <c r="C11" s="9" t="s">
+      <c r="C11" s="5" t="s">
         <v>17</v>
       </c>
-      <c r="D11" s="8" t="s">
-        <v>8</v>
-      </c>
-      <c r="E11" s="10">
+      <c r="D11" s="4" t="s">
+        <v>8</v>
+      </c>
+      <c r="E11" s="6">
         <v>4</v>
       </c>
-      <c r="F11" s="11" t="s">
+      <c r="F11" s="7" t="s">
         <v>7</v>
       </c>
     </row>
     <row r="12" spans="1:6" x14ac:dyDescent="1">
-      <c r="A12" s="8">
-        <v>8</v>
-      </c>
-      <c r="B12" s="9" t="s">
+      <c r="A12" s="4">
+        <v>8</v>
+      </c>
+      <c r="B12" s="5" t="s">
         <v>30</v>
       </c>
-      <c r="C12" s="9" t="s">
+      <c r="C12" s="5" t="s">
         <v>18</v>
       </c>
-      <c r="D12" s="8" t="s">
-        <v>8</v>
-      </c>
-      <c r="E12" s="10">
+      <c r="D12" s="4" t="s">
+        <v>8</v>
+      </c>
+      <c r="E12" s="6">
         <v>2</v>
       </c>
-      <c r="F12" s="11" t="s">
+      <c r="F12" s="7" t="s">
         <v>7</v>
       </c>
     </row>
     <row r="13" spans="1:6" x14ac:dyDescent="1">
-      <c r="A13" s="8">
+      <c r="A13" s="4">
         <v>9</v>
       </c>
-      <c r="B13" s="9" t="s">
+      <c r="B13" s="5" t="s">
         <v>33</v>
       </c>
-      <c r="C13" s="9" t="s">
+      <c r="C13" s="5" t="s">
         <v>34</v>
       </c>
-      <c r="D13" s="8" t="s">
-        <v>8</v>
-      </c>
-      <c r="E13" s="10">
+      <c r="D13" s="4" t="s">
+        <v>8</v>
+      </c>
+      <c r="E13" s="6">
         <v>3</v>
       </c>
-      <c r="F13" s="11" t="s">
+      <c r="F13" s="7" t="s">
         <v>7</v>
       </c>
     </row>
     <row r="14" spans="1:6" x14ac:dyDescent="1">
-      <c r="A14" s="8">
+      <c r="A14" s="4">
         <v>10</v>
       </c>
-      <c r="B14" s="9" t="s">
+      <c r="B14" s="5" t="s">
         <v>40</v>
       </c>
-      <c r="C14" s="9" t="s">
+      <c r="C14" s="5" t="s">
         <v>39</v>
       </c>
-      <c r="D14" s="8" t="s">
+      <c r="D14" s="4" t="s">
         <v>6</v>
       </c>
-      <c r="E14" s="10">
+      <c r="E14" s="6">
         <v>4</v>
       </c>
-      <c r="F14" s="11" t="s">
+      <c r="F14" s="7" t="s">
         <v>7</v>
       </c>
     </row>
     <row r="15" spans="1:6" x14ac:dyDescent="1">
-      <c r="A15" s="8">
+      <c r="A15" s="4">
         <v>11</v>
       </c>
-      <c r="B15" s="9" t="s">
+      <c r="B15" s="5" t="s">
         <v>36</v>
       </c>
-      <c r="C15" s="9" t="s">
+      <c r="C15" s="5" t="s">
         <v>35</v>
       </c>
-      <c r="D15" s="8" t="s">
+      <c r="D15" s="4" t="s">
         <v>6</v>
       </c>
-      <c r="E15" s="10">
+      <c r="E15" s="6">
         <v>3</v>
       </c>
-      <c r="F15" s="11" t="s">
+      <c r="F15" s="7" t="s">
         <v>7</v>
       </c>
     </row>
     <row r="16" spans="1:6" x14ac:dyDescent="1">
-      <c r="A16" s="8">
+      <c r="A16" s="4">
         <v>12</v>
       </c>
-      <c r="B16" s="9" t="s">
+      <c r="B16" s="5" t="s">
         <v>41</v>
       </c>
-      <c r="C16" s="9" t="s">
+      <c r="C16" s="5" t="s">
         <v>42</v>
       </c>
-      <c r="D16" s="8" t="s">
-        <v>8</v>
-      </c>
-      <c r="E16" s="10">
+      <c r="D16" s="4" t="s">
+        <v>8</v>
+      </c>
+      <c r="E16" s="6">
         <v>1</v>
       </c>
-      <c r="F16" s="11" t="s">
+      <c r="F16" s="7" t="s">
         <v>7</v>
       </c>
     </row>
     <row r="17" spans="1:6" x14ac:dyDescent="1">
-      <c r="A17" s="8">
+      <c r="A17" s="4">
         <v>13</v>
       </c>
-      <c r="B17" s="9" t="s">
+      <c r="B17" s="5" t="s">
         <v>45</v>
       </c>
-      <c r="C17" s="9" t="s">
+      <c r="C17" s="5" t="s">
         <v>46</v>
       </c>
-      <c r="D17" s="8" t="s">
+      <c r="D17" s="4" t="s">
         <v>6</v>
       </c>
-      <c r="E17" s="10">
+      <c r="E17" s="6">
         <v>1</v>
       </c>
-      <c r="F17" s="11" t="s">
+      <c r="F17" s="7" t="s">
         <v>7</v>
       </c>
     </row>
     <row r="18" spans="1:6" x14ac:dyDescent="1">
-      <c r="A18" s="8">
+      <c r="A18" s="4">
         <v>14</v>
       </c>
-      <c r="B18" s="9" t="s">
+      <c r="B18" s="5" t="s">
         <v>37</v>
       </c>
-      <c r="C18" s="9" t="s">
+      <c r="C18" s="5" t="s">
         <v>38</v>
       </c>
-      <c r="D18" s="8" t="s">
+      <c r="D18" s="4" t="s">
         <v>6</v>
       </c>
-      <c r="E18" s="10">
+      <c r="E18" s="6">
         <v>5</v>
       </c>
-      <c r="F18" s="11" t="s">
+      <c r="F18" s="7" t="s">
         <v>7</v>
       </c>
     </row>
     <row r="19" spans="1:6" x14ac:dyDescent="1">
-      <c r="A19" s="8">
+      <c r="A19" s="4">
         <v>15</v>
       </c>
-      <c r="B19" s="9" t="s">
+      <c r="B19" s="5" t="s">
         <v>43</v>
       </c>
-      <c r="C19" s="9" t="s">
+      <c r="C19" s="5" t="s">
         <v>44</v>
       </c>
-      <c r="D19" s="8" t="s">
-        <v>8</v>
-      </c>
-      <c r="E19" s="10">
+      <c r="D19" s="4" t="s">
+        <v>8</v>
+      </c>
+      <c r="E19" s="6">
         <v>2</v>
       </c>
-      <c r="F19" s="11" t="s">
+      <c r="F19" s="7" t="s">
         <v>7</v>
       </c>
     </row>
     <row r="20" spans="1:6" x14ac:dyDescent="1">
-      <c r="A20" s="8">
+      <c r="A20" s="4">
         <v>16</v>
       </c>
-      <c r="B20" s="9" t="s">
+      <c r="B20" s="5" t="s">
         <v>47</v>
       </c>
-      <c r="C20" s="9" t="s">
+      <c r="C20" s="5" t="s">
         <v>48</v>
       </c>
-      <c r="D20" s="8" t="s">
-        <v>8</v>
-      </c>
-      <c r="E20" s="10">
+      <c r="D20" s="4" t="s">
+        <v>8</v>
+      </c>
+      <c r="E20" s="6">
         <v>1</v>
       </c>
-      <c r="F20" s="11" t="s">
+      <c r="F20" s="7" t="s">
         <v>7</v>
       </c>
     </row>
     <row r="21" spans="1:6" x14ac:dyDescent="1">
-      <c r="A21" s="8">
+      <c r="A21" s="4">
         <v>17</v>
       </c>
-      <c r="B21" s="12" t="s">
+      <c r="B21" s="5" t="s">
+        <v>50</v>
+      </c>
+      <c r="C21" s="5" t="s">
+        <v>49</v>
+      </c>
+      <c r="D21" s="4" t="s">
+        <v>6</v>
+      </c>
+      <c r="E21" s="6">
+        <v>5</v>
+      </c>
+      <c r="F21" s="7" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="22" spans="1:6" x14ac:dyDescent="1">
+      <c r="A22" s="4">
+        <v>18</v>
+      </c>
+      <c r="B22" s="5" t="s">
+        <v>51</v>
+      </c>
+      <c r="C22" s="5" t="s">
+        <v>52</v>
+      </c>
+      <c r="D22" s="4" t="s">
+        <v>8</v>
+      </c>
+      <c r="E22" s="6">
+        <v>8</v>
+      </c>
+      <c r="F22" s="7"/>
+    </row>
+    <row r="23" spans="1:6" x14ac:dyDescent="1">
+      <c r="A23" s="4">
+        <v>19</v>
+      </c>
+      <c r="B23" s="8" t="s">
         <v>32</v>
       </c>
-      <c r="C21" s="9" t="s">
+      <c r="C23" s="5" t="s">
         <v>19</v>
       </c>
-      <c r="D21" s="8" t="s">
+      <c r="D23" s="4" t="s">
         <v>20</v>
       </c>
-      <c r="E21" s="10">
-        <v>12</v>
-      </c>
-      <c r="F21" s="12" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="22" spans="1:6" x14ac:dyDescent="1">
-      <c r="A22" s="8">
-        <v>18</v>
-      </c>
-      <c r="B22" s="9" t="s">
+      <c r="E23" s="6">
+        <v>14</v>
+      </c>
+      <c r="F23" s="8" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="24" spans="1:6" x14ac:dyDescent="1">
+      <c r="A24" s="4">
+        <v>20</v>
+      </c>
+      <c r="B24" s="5" t="s">
         <v>31</v>
       </c>
-      <c r="C22" s="9" t="s">
+      <c r="C24" s="5" t="s">
         <v>21</v>
       </c>
-      <c r="D22" s="8" t="s">
+      <c r="D24" s="4" t="s">
         <v>22</v>
       </c>
-      <c r="E22" s="10">
+      <c r="E24" s="6">
         <v>6</v>
       </c>
-      <c r="F22" s="11" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="23" spans="1:6" x14ac:dyDescent="1">
-      <c r="A23" s="13"/>
-      <c r="B23" s="13"/>
-      <c r="C23" s="13"/>
-      <c r="D23" s="14" t="s">
+      <c r="F24" s="7" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="25" spans="1:6" x14ac:dyDescent="1">
+      <c r="A25" s="9"/>
+      <c r="B25" s="9"/>
+      <c r="C25" s="9"/>
+      <c r="D25" s="10" t="s">
         <v>9</v>
       </c>
-      <c r="E23" s="14">
-        <f>SUM(E5:E22)</f>
-        <v>75</v>
-      </c>
-      <c r="F23" s="11"/>
+      <c r="E25" s="10">
+        <f>SUM(E5:E24)</f>
+        <v>90</v>
+      </c>
+      <c r="F25" s="7"/>
     </row>
   </sheetData>
   <mergeCells count="2">

</xml_diff>